<commit_message>
Exploring charts with Excel loaded data.
</commit_message>
<xml_diff>
--- a/adt_data.xlsx
+++ b/adt_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="CV115_Abertas" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>ANO_MES</t>
   </si>
@@ -410,11 +410,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="127356928"/>
-        <c:axId val="127277248"/>
+        <c:axId val="213704704"/>
+        <c:axId val="149983744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127356928"/>
+        <c:axId val="213704704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -424,7 +424,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127277248"/>
+        <c:crossAx val="149983744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -432,7 +432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127277248"/>
+        <c:axId val="149983744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127356928"/>
+        <c:crossAx val="213704704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -624,11 +624,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="128590336"/>
-        <c:axId val="126422976"/>
+        <c:axId val="213706752"/>
+        <c:axId val="149986048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128590336"/>
+        <c:axId val="213706752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126422976"/>
+        <c:crossAx val="149986048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,7 +646,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126422976"/>
+        <c:axId val="149986048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +657,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128590336"/>
+        <c:crossAx val="213706752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -948,11 +948,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="134382592"/>
-        <c:axId val="191447040"/>
+        <c:axId val="175845376"/>
+        <c:axId val="213631552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134382592"/>
+        <c:axId val="175845376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191447040"/>
+        <c:crossAx val="213631552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -970,7 +970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191447040"/>
+        <c:axId val="213631552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134382592"/>
+        <c:crossAx val="175845376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1395,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:O24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,147 +1803,6 @@
       </c>
       <c r="O21" s="3">
         <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>3</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>4</v>
-      </c>
-      <c r="M22">
-        <v>7</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23">
-        <v>2</v>
-      </c>
-      <c r="J23" t="s">
-        <v>5</v>
-      </c>
-      <c r="K23">
-        <v>4</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>25</v>
-      </c>
-      <c r="D24">
-        <v>26</v>
-      </c>
-      <c r="E24">
-        <v>34</v>
-      </c>
-      <c r="F24">
-        <v>47</v>
-      </c>
-      <c r="G24">
-        <v>19</v>
-      </c>
-      <c r="H24">
-        <v>19</v>
-      </c>
-      <c r="I24">
-        <v>29</v>
-      </c>
-      <c r="J24">
-        <v>12</v>
-      </c>
-      <c r="K24">
-        <v>8</v>
-      </c>
-      <c r="L24">
-        <v>6</v>
-      </c>
-      <c r="M24">
-        <v>5</v>
-      </c>
-      <c r="N24">
-        <v>5</v>
-      </c>
-      <c r="O24">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2196,7 +2055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>

</xml_diff>